<commit_message>
Added test to write data to excel and json
</commit_message>
<xml_diff>
--- a/src/main/java/data/testdata.xlsx
+++ b/src/main/java/data/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajat\IdeaProjects\untitled\src\main\java\data\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -42,12 +42,25 @@
   </si>
   <si>
     <t>abcfghkljedi</t>
+  </si>
+  <si>
+    <t>test@example.com</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>tester@ample.com</t>
+  </si>
+  <si>
+    <t>password754</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -392,8 +405,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -418,6 +431,30 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor modifications for reporting
</commit_message>
<xml_diff>
--- a/src/main/java/data/testdata.xlsx
+++ b/src/main/java/data/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -489,6 +489,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>